<commit_message>
input file and output file
</commit_message>
<xml_diff>
--- a/MHSP/data/House_Info.xlsx
+++ b/MHSP/data/House_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shengyc\Documents\GitHub\Long_Term_Housing_Planning\MHSP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yin\Desktop\bay\Long-Term_MHSP\Long_Term_Housing_Planning\MHSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03B63E8-5065-40DA-A242-F29E33C95C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA224AE4-B57D-4D1F-AD15-08D240C8F7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="29760" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Type</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>Trailer</t>
-  </si>
-  <si>
-    <t>r_p</t>
-  </si>
-  <si>
-    <t>H_p</t>
   </si>
 </sst>
 </file>
@@ -377,21 +371,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,7 +396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -413,7 +407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -422,28 +416,6 @@
       </c>
       <c r="C3" s="1">
         <v>69000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>